<commit_message>
Fixed typos in manuscript, and example notebooks
</commit_message>
<xml_diff>
--- a/Examples/Liquid, Ol_Liq_Themometry/Thermometry_out.xlsx
+++ b/Examples/Liquid, Ol_Liq_Themometry/Thermometry_out.xlsx
@@ -52,7 +52,7 @@
     <t>H2O_Liq</t>
   </si>
   <si>
-    <t>Fe3FeT_Liq</t>
+    <t>Fe3Fet_Liq</t>
   </si>
   <si>
     <t>NiO_Liq</t>
@@ -540,7 +540,7 @@
         <v>5.59000015258789</v>
       </c>
       <c r="N2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -605,7 +605,7 @@
         <v>6.55000019073486</v>
       </c>
       <c r="N3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>3.14000010490418</v>
       </c>
       <c r="N4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>6.19999980926514</v>
       </c>
       <c r="N5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>6.57999992370606</v>
       </c>
       <c r="N6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>6.80999994277954</v>
       </c>
       <c r="N7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>6.46000003814697</v>
       </c>
       <c r="N8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -995,7 +995,7 @@
         <v>14.2399997711182</v>
       </c>
       <c r="N9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>14.3400001525879</v>
       </c>
       <c r="N10">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>5.15999984741211</v>
       </c>
       <c r="N11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>0</v>

</xml_diff>

<commit_message>
updated examples to use pip
</commit_message>
<xml_diff>
--- a/Examples/Liquid, Ol_Liq_Themometry/Thermometry_out.xlsx
+++ b/Examples/Liquid, Ol_Liq_Themometry/Thermometry_out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>SiO2_Liq</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Sample_ID_Liq</t>
-  </si>
-  <si>
-    <t>P_kbar</t>
   </si>
   <si>
     <t>Teq15_2H2O</t>
@@ -431,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,11 +492,8 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -555,16 +549,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>1108.710016820756</v>
       </c>
       <c r="T2">
-        <v>1108.710016820756</v>
-      </c>
-      <c r="U2">
         <v>1083.050016820756</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -620,16 +611,13 @@
         <v>1</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>1069.891842359795</v>
       </c>
       <c r="T3">
-        <v>1069.891842359795</v>
-      </c>
-      <c r="U3">
         <v>1044.231842359795</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -685,16 +673,13 @@
         <v>2</v>
       </c>
       <c r="S4">
-        <v>5</v>
+        <v>1060.765739361339</v>
       </c>
       <c r="T4">
-        <v>1060.765739361339</v>
-      </c>
-      <c r="U4">
         <v>1035.105739361339</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -750,16 +735,13 @@
         <v>3</v>
       </c>
       <c r="S5">
-        <v>5</v>
+        <v>1025.950726039591</v>
       </c>
       <c r="T5">
-        <v>1025.950726039591</v>
-      </c>
-      <c r="U5">
         <v>1000.290726039591</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -815,16 +797,13 @@
         <v>4</v>
       </c>
       <c r="S6">
-        <v>5</v>
+        <v>1088.635168266626</v>
       </c>
       <c r="T6">
-        <v>1088.635168266626</v>
-      </c>
-      <c r="U6">
         <v>1062.975168266626</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -880,16 +859,13 @@
         <v>5</v>
       </c>
       <c r="S7">
-        <v>5</v>
+        <v>1075.714112517679</v>
       </c>
       <c r="T7">
-        <v>1075.714112517679</v>
-      </c>
-      <c r="U7">
         <v>1050.05411251768</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -945,16 +921,13 @@
         <v>6</v>
       </c>
       <c r="S8">
-        <v>5</v>
+        <v>1058.655371277641</v>
       </c>
       <c r="T8">
-        <v>1058.655371277641</v>
-      </c>
-      <c r="U8">
         <v>1032.995371277641</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1010,16 +983,13 @@
         <v>7</v>
       </c>
       <c r="S9">
-        <v>5</v>
+        <v>1083.961042688784</v>
       </c>
       <c r="T9">
-        <v>1083.961042688784</v>
-      </c>
-      <c r="U9">
         <v>1058.301042688784</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1075,16 +1045,13 @@
         <v>8</v>
       </c>
       <c r="S10">
-        <v>5</v>
+        <v>1058.281402120356</v>
       </c>
       <c r="T10">
-        <v>1058.281402120356</v>
-      </c>
-      <c r="U10">
         <v>1032.621402120356</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1140,12 +1107,9 @@
         <v>9</v>
       </c>
       <c r="S11">
-        <v>5</v>
+        <v>1129.211251997238</v>
       </c>
       <c r="T11">
-        <v>1129.211251997238</v>
-      </c>
-      <c r="U11">
         <v>1103.551251997238</v>
       </c>
     </row>

</xml_diff>